<commit_message>
TradingModel - 2021/11/11 data update / 個股歷史損益 / 每日歷史總損益 / 完成
</commit_message>
<xml_diff>
--- a/TradingModel_OpenPositionTodayClose.xlsx
+++ b/TradingModel_OpenPositionTodayClose.xlsx
@@ -461,7 +461,7 @@
         <v>-5973</v>
       </c>
       <c r="D2" t="n">
-        <v>29.4</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="3">
@@ -469,13 +469,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3035</v>
+        <v>3033</v>
       </c>
       <c r="C3" t="n">
-        <v>-5920</v>
+        <v>-5850</v>
       </c>
       <c r="D3" t="n">
-        <v>194</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -483,15 +483,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3141</v>
+        <v>3035</v>
       </c>
       <c r="C4" t="n">
-        <v>-5899.5</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>233.50</t>
-        </is>
+        <v>-5920</v>
+      </c>
+      <c r="D4" t="n">
+        <v>191</v>
       </c>
     </row>
     <row r="5">
@@ -499,13 +497,15 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3189</v>
+        <v>3141</v>
       </c>
       <c r="C5" t="n">
-        <v>-6345</v>
-      </c>
-      <c r="D5" t="n">
-        <v>250</v>
+        <v>-5899.5</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>256.50</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -513,34 +513,32 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3504</v>
+        <v>3189</v>
       </c>
       <c r="C6" t="n">
-        <v>-5934</v>
+        <v>-6345</v>
       </c>
       <c r="D6" t="n">
-        <v>133.5</v>
+        <v>243.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>6170</v>
+        <v>3504</v>
       </c>
       <c r="C7" t="n">
-        <v>-6201</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>48.10</t>
-        </is>
+        <v>-5934</v>
+      </c>
+      <c r="D7" t="n">
+        <v>130</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
         <v>6411</v>
@@ -550,7 +548,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>234.00</t>
+          <t>257.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
TradingModel - 2021/11/12 data update
</commit_message>
<xml_diff>
--- a/TradingModel_OpenPositionTodayClose.xlsx
+++ b/TradingModel_OpenPositionTodayClose.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,11 +441,6 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EachCalculateProfit</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>TodayClose</t>
         </is>
       </c>
@@ -458,10 +453,7 @@
         <v>1711</v>
       </c>
       <c r="C2" t="n">
-        <v>-5973</v>
-      </c>
-      <c r="D2" t="n">
-        <v>28.5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -469,13 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3033</v>
+        <v>2436</v>
       </c>
       <c r="C3" t="n">
-        <v>-5850</v>
-      </c>
-      <c r="D3" t="n">
-        <v>31</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="4">
@@ -483,13 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3035</v>
+        <v>3033</v>
       </c>
       <c r="C4" t="n">
-        <v>-5920</v>
-      </c>
-      <c r="D4" t="n">
-        <v>191</v>
+        <v>31.65</v>
       </c>
     </row>
     <row r="5">
@@ -497,15 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3141</v>
+        <v>3035</v>
       </c>
       <c r="C5" t="n">
-        <v>-5899.5</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>256.50</t>
-        </is>
+        <v>189</v>
       </c>
     </row>
     <row r="6">
@@ -513,13 +494,12 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3189</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-6345</v>
-      </c>
-      <c r="D6" t="n">
-        <v>243.5</v>
+        <v>3141</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>267.00</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -527,28 +507,46 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>3504</v>
+        <v>3189</v>
       </c>
       <c r="C7" t="n">
-        <v>-5934</v>
-      </c>
-      <c r="D7" t="n">
-        <v>130</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
+        <v>3588</v>
+      </c>
+      <c r="C8" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>6104</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>165.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
         <v>6411</v>
       </c>
-      <c r="C8" t="n">
-        <v>-5980</v>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
-          <t>257.00</t>
+          <t>264.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
TradingModel - 2021/11/15 data update
</commit_message>
<xml_diff>
--- a/TradingModel_OpenPositionTodayClose.xlsx
+++ b/TradingModel_OpenPositionTodayClose.xlsx
@@ -447,106 +447,110 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1711</v>
+        <v>2436</v>
       </c>
       <c r="C2" t="n">
-        <v>28</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>2436</v>
+        <v>3035</v>
       </c>
       <c r="C3" t="n">
-        <v>102.5</v>
+        <v>198.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>3033</v>
-      </c>
-      <c r="C4" t="n">
-        <v>31.65</v>
+        <v>3122</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>66.80</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>3035</v>
-      </c>
-      <c r="C5" t="n">
-        <v>189</v>
+        <v>3141</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>251.50</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>3141</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>267.00</t>
-        </is>
+        <v>3588</v>
+      </c>
+      <c r="C6" t="n">
+        <v>163</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>3189</v>
-      </c>
-      <c r="C7" t="n">
-        <v>251</v>
+        <v>6104</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>182.00</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>3588</v>
-      </c>
-      <c r="C8" t="n">
-        <v>161</v>
+        <v>6138</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>213.00</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>6104</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>165.50</t>
-        </is>
+        <v>6271</v>
+      </c>
+      <c r="C9" t="n">
+        <v>302.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="n">
         <v>6411</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>264.00</t>
+          <t>290.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
TradingModel - 2021/11/16 data update / Remove `Check`
</commit_message>
<xml_diff>
--- a/TradingModel_OpenPositionTodayClose.xlsx
+++ b/TradingModel_OpenPositionTodayClose.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,21 +450,21 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2436</v>
+        <v>2314</v>
       </c>
       <c r="C2" t="n">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3035</v>
+        <v>2436</v>
       </c>
       <c r="C3" t="n">
-        <v>198.5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
@@ -472,12 +472,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>3122</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>66.80</t>
-        </is>
+        <v>3035</v>
+      </c>
+      <c r="C4" t="n">
+        <v>193.5</v>
       </c>
     </row>
     <row r="5">
@@ -485,72 +483,111 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>3141</v>
+        <v>3122</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>251.50</t>
+          <t>67.40</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>3588</v>
-      </c>
-      <c r="C6" t="n">
-        <v>163</v>
+        <v>3141</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>242.50</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>6104</v>
+        <v>3221</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>182.00</t>
+          <t>43.10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>6138</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>213.00</t>
-        </is>
+        <v>3588</v>
+      </c>
+      <c r="C8" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>6271</v>
-      </c>
-      <c r="C9" t="n">
-        <v>302.5</v>
+        <v>6104</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>179.00</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="n">
+        <v>6138</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>214.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B11" t="n">
+        <v>6271</v>
+      </c>
+      <c r="C11" t="n">
+        <v>300.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B12" t="n">
         <v>6411</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>290.00</t>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>268.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B13" t="n">
+        <v>8289</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>36.95</t>
         </is>
       </c>
     </row>

</xml_diff>